<commit_message>
Debugging issues with error table testing
</commit_message>
<xml_diff>
--- a/Gbat_Testing/Excel_F1A/F1A.xlsx
+++ b/Gbat_Testing/Excel_F1A/F1A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\VSprojects\gbat\Gbat_Testing\Excel_F1A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\VSprojects\Gbat-Testing\Gbat_Testing\Excel_F1A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC7AB1A-35A8-4945-8D59-E6FD47E9609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A030A0-33F5-46F8-8DED-1C003A0299B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBatch" sheetId="1" r:id="rId1"/>
@@ -1421,7 +1421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA03B96-3D48-47CE-AB75-C07683954905}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2274,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6265FDB6-BB18-4AB3-A2EC-7AF80649CB0C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Draft of api request for inputs
</commit_message>
<xml_diff>
--- a/Gbat_Testing/Excel_F1A/F1A.xlsx
+++ b/Gbat_Testing/Excel_F1A/F1A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\VSprojects\Gbat-Testing\Gbat_Testing\Excel_F1A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A030A0-33F5-46F8-8DED-1C003A0299B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31641F59-60FD-44E8-97AA-7708BA875626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBatch" sheetId="1" r:id="rId1"/>
@@ -847,14 +847,14 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -992,7 +992,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B1" sqref="B1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA03B96-3D48-47CE-AB75-C07683954905}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on automating error test
</commit_message>
<xml_diff>
--- a/Gbat_Testing/Excel_F1A/F1A.xlsx
+++ b/Gbat_Testing/Excel_F1A/F1A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\VSprojects\Gbat-Testing\Gbat_Testing\Excel_F1A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31641F59-60FD-44E8-97AA-7708BA875626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27318ED4-426C-4076-AE43-B9836E1B9ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestBatch" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="150">
   <si>
     <t>boro</t>
   </si>
@@ -847,7 +847,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA03B96-3D48-47CE-AB75-C07683954905}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,9 +1562,7 @@
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>88</v>
       </c>

</xml_diff>